<commit_message>
General updates to folder
</commit_message>
<xml_diff>
--- a/stat_tests/combined_anova_data_edited.xlsx
+++ b/stat_tests/combined_anova_data_edited.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yasminebassil/Documents/Emory/3_Research/Projects/CogMap_Paper/stat_tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0FBA304C-5AF4-9D42-AAB8-1B162B9E53DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C3574631-53FD-7C49-9412-52C6E417B471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="combined_anova_data" sheetId="1" r:id="rId1"/>
@@ -230,7 +230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -410,8 +410,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <start/>
       <end/>
@@ -526,6 +532,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <start/>
+      <end/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -571,9 +586,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -652,11 +671,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -672,11 +691,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -993,7 +1012,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E31"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1595,260 +1614,260 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" s="4">
         <v>162.80177277267799</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="4">
         <v>81.400886386338897</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="4">
         <v>2</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="4">
         <v>575.00000046199602</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="4">
         <v>11.890524065087501</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="5">
         <v>8.7084744571134005E-6</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23" s="5">
         <f>F23*3</f>
         <v>2.6125423371340201E-5</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="A24" s="2">
         <v>123.86767556497399</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <v>17.695382223567702</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="2">
         <v>7</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="2">
         <v>575.00000064231801</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <v>2.5848289559358602</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>1.24663800726111E-2</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="2">
         <f t="shared" ref="H24:H31" si="1">F24*3</f>
         <v>3.7399140217833304E-2</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" s="2">
         <v>140.57152957435</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <v>10.040823541025</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="2">
         <v>14</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="2">
         <v>575.00000062971606</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <v>1.46669967918054</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>0.118460490772683</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="2">
         <f t="shared" si="1"/>
         <v>0.35538147231804901</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="2">
         <v>10743.187169274601</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="2">
         <v>5371.5935846372904</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2">
         <v>2</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="2">
         <v>575.00000035052597</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <v>6.0541410626985899</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="2">
         <v>2.5004655581663902E-3</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="2">
         <f t="shared" si="1"/>
         <v>7.5013966744991705E-3</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="A27" s="2">
         <v>220881.79384292199</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="2">
         <v>31554.5419775603</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="2">
         <v>7</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="2">
         <v>575.00000045601803</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="2">
         <v>35.564054742963897</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27" s="3">
         <v>2.65515673362228E-41</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H27" s="3">
         <f t="shared" si="1"/>
         <v>7.9654702008668401E-41</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="A28" s="2">
         <v>21050.201614454101</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="2">
         <v>1503.58582960386</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="2">
         <v>14</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="2">
         <v>575.00000040069403</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="2">
         <v>1.69464062551767</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="2">
         <v>5.2752173462790403E-2</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="2">
         <f t="shared" si="1"/>
         <v>0.15825652038837121</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="A29" s="2">
         <v>29.732228080954499</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="2">
         <v>14.8661140404772</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="2">
         <v>2</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="2">
         <v>575.00000065548204</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="2">
         <v>10.481914978784699</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="3">
         <v>3.37896260059461E-5</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29" s="3">
         <f t="shared" si="1"/>
         <v>1.0136887801783829E-4</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="A30" s="2">
         <v>144.23058262501101</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="2">
         <v>20.604368946430199</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="2">
         <v>7</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="2">
         <v>575.00000062638401</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="2">
         <v>14.527888249743301</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30" s="3">
         <v>1.82697826974788E-17</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30" s="3">
         <f t="shared" si="1"/>
         <v>5.4809348092436399E-17</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="A31" s="2">
         <v>29.012901234530201</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="2">
         <v>2.07235008818073</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="2">
         <v>14</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="2">
         <v>575.00000063871505</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="2">
         <v>1.4611886718642499</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="2">
         <v>0.120672301527943</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="2">
         <f t="shared" si="1"/>
         <v>0.36201690458382901</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
-      <formula>0.001</formula>
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="between">
+      <formula>0.05</formula>
+      <formula>0.01</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
       <formula>0.01</formula>
       <formula>0.001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
-      <formula>0.05</formula>
-      <formula>0.01</formula>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="lessThan">
+      <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">

</xml_diff>